<commit_message>
start of spring 2021 and grade change materials
</commit_message>
<xml_diff>
--- a/FALL 2020/CSE 201/results/jan26/SaD_203_CSE201_2_with_MarksDistribution.xlsx
+++ b/FALL 2020/CSE 201/results/jan26/SaD_203_CSE201_2_with_MarksDistribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 2020\CSE 201\results\jan26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09E89F-30E2-402B-AD1C-33D9E304B5A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249B5EF7-36CB-4104-B024-9391D306747B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GradeSheet" sheetId="1" r:id="rId1"/>
@@ -930,13 +930,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1407,8 +1407,8 @@
   </sheetPr>
   <dimension ref="A1:W1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1"/>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="D27" s="27">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E27" s="45">
         <f>ROUNDUP(((O27)/(O$9))*GradeSheet!$C$45,0)</f>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="F27" s="45">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G27" s="46">
         <f t="shared" si="4"/>
@@ -2979,26 +2979,26 @@
       </c>
       <c r="I27" s="47">
         <f t="shared" si="6"/>
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="J27" s="48">
         <f t="shared" ref="J27:J36" si="8">I27/100</f>
-        <v>0.39</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K27" s="49" t="str">
         <f>VLOOKUP(I27,GradingPolicy!$B$2:$C$11,2)</f>
-        <v>F (Fail)</v>
+        <v>C (Plain)</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="27">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O27" s="27">
         <v>9</v>
       </c>
       <c r="P27" s="27">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q27" s="27">
         <v>15</v>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="P44" s="25">
         <f>MAX(P10:P40)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q44" s="25">
         <f>MAX(Q10:Q40)</f>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="N45" s="25">
         <f>AVERAGE(N10:N40)</f>
-        <v>9.4516129032258061</v>
+        <v>9.7096774193548381</v>
       </c>
       <c r="O45" s="25">
         <f>AVERAGE(O10:O40)</f>
@@ -4114,7 +4114,7 @@
       </c>
       <c r="P45" s="25">
         <f>AVERAGE(P10:P40)</f>
-        <v>9.5161290322580641</v>
+        <v>9.7741935483870961</v>
       </c>
       <c r="Q45" s="25">
         <f>AVERAGE(Q10:Q40)</f>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="G51" s="26">
         <f>COUNTIF(K10:K40, "C (Plain)")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="G53" s="26">
         <f>COUNTIF(K10:K40, "F (Fail)")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -16854,7 +16854,7 @@
       </c>
       <c r="B18" s="57" t="str">
         <f>VLOOKUP(GradeSheet!$K27,GradingPolicy!$C$2:$D$11,2,FALSE)</f>
-        <v>F</v>
+        <v>C</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.6">

</xml_diff>

<commit_message>
added grade change forms
</commit_message>
<xml_diff>
--- a/FALL 2020/CSE 201/results/jan26/SaD_203_CSE201_2_with_MarksDistribution.xlsx
+++ b/FALL 2020/CSE 201/results/jan26/SaD_203_CSE201_2_with_MarksDistribution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 2020\CSE 201\results\jan26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249B5EF7-36CB-4104-B024-9391D306747B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64532D24-731B-43F2-81B2-6C466328F396}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="744" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GradeSheet" sheetId="1" r:id="rId1"/>
@@ -1407,8 +1407,8 @@
   </sheetPr>
   <dimension ref="A1:W1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1"/>
@@ -16997,8 +16997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11239E0C-BAAE-4C30-B1FF-E4D9A9015B81}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I22" activeCellId="1" sqref="I18 I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4"/>

</xml_diff>